<commit_message>
modified model simulation and subsequent processing to include condition-specific variability, added simulation to estimate earnings based on model estimated and average aim points
</commit_message>
<xml_diff>
--- a/Taraz_prelim.xlsx
+++ b/Taraz_prelim.xlsx
@@ -15,9 +15,9 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
     <sheet name="model_AICs_by_condition" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -2184,7 +2184,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A41:F43" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="10">
     <pivotField dataField="1" showAll="0"/>
@@ -2278,7 +2278,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A25:C38" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField showAll="0"/>
@@ -2402,7 +2402,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A4:J19" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="10">
     <pivotField dataField="1" showAll="0"/>

</xml_diff>